<commit_message>
Avance de Proyectos del Visual Studio
Se crearon nuevos proyectos para la solucion
</commit_message>
<xml_diff>
--- a/Recursos/Datos financieros.xlsx
+++ b/Recursos/Datos financieros.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\UDB\Ciclo 05 2024\Datawarehouse y Minería de Datos DMD941\Unidad 3\Proyecto Fase 1\Recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\UDB\Ciclo 05 2024\Datawarehouse y Minería de Datos DMD941\Unidad 3\Proyecto Fase 1\DMD_Proyecto\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B2285B-5889-4D94-B0B5-E198630D92CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8705C7A-FD93-4E0C-A536-90A862A956E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,6 +257,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -274,7 +275,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -530,8 +530,8 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Beneficio" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fecha" dataDxfId="3"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Número de mes" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Nombre de mes" dataDxfId="0"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Año" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Nombre de mes" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Año" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -803,7 +803,7 @@
   <dimension ref="A1:P701"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P701"/>
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35889,6 +35889,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002914170AD08CD84791A27D153F5B634B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5429c1527982b506b3a2dcd5af97d528">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e53ec00ec453a1eec4584499b9bdd29">
     <xsd:element name="properties">
@@ -36002,21 +36017,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5211F8-A83C-4A0E-89EA-EB022F37C477}">
   <ds:schemaRefs>
@@ -36026,6 +36026,29 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36101D31-F691-4436-A911-BDE8158BB67A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A11FD15B-C292-4476-9AA9-A2FF2D0A22B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E22C849-2538-4665-AED1-7E13010FACF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36039,27 +36062,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A11FD15B-C292-4476-9AA9-A2FF2D0A22B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36101D31-F691-4436-A911-BDE8158BB67A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>